<commit_message>
uploading excel file now notifies whether it was success or failure.
</commit_message>
<xml_diff>
--- a/rooms.xlsx
+++ b/rooms.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zaura\IdeaProjects\SmartCampus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13272" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
   <si>
     <t>ამფითეატრი</t>
   </si>
@@ -195,7 +196,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Sylfaen"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
         <scheme val="minor"/>
@@ -307,6 +308,9 @@
   </si>
   <si>
     <t>ტიპი</t>
+  </si>
+  <si>
+    <t>104ა</t>
   </si>
 </sst>
 </file>
@@ -317,7 +321,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Sylfaen"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
@@ -667,16 +671,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121:C121"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.6">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -2000,4 +2004,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>